<commit_message>
* Adapt blancofw v3.x * fix some generics errors on IntelliJ.
</commit_message>
<xml_diff>
--- a/meta/validators/ValidateConfig.xlsx
+++ b/meta/validators/ValidateConfig.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10514"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/dapanda/dapanda-front-core/meta/validators/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tueda/data/webstorm/atr/api/atrcall-front-app/meta/validators/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59915E94-2F2A-6244-8305-C24374EEF05E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CAD90BC-84FB-0840-84A2-959E94FF72ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24320" yWindow="2800" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8800" yWindow="6020" windowWidth="25200" windowHeight="17540" tabRatio="640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="validate" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="67">
   <si>
     <t>パッケージ</t>
   </si>
@@ -463,15 +463,19 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>import {I18n, VueMessageType} from "vue-i18n"</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>import { LocaleMessageDictionary, LocaleMessages } from "@intlify/core-base"</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>validators</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import { I18n } from "vue-i18n"</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>import { DapandaI18nResources } from "@/i18n/DapandaMessages"</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -1201,27 +1205,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1235,22 +1238,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1262,8 +1258,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1293,18 +1289,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1318,22 +1312,22 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1362,16 +1356,7 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="49" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1379,6 +1364,33 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1400,44 +1412,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1850,10 +1835,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L48"/>
+  <dimension ref="A1:L49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14"/>
@@ -1895,8 +1880,6 @@
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="5"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
@@ -1908,11 +1891,9 @@
       </c>
       <c r="D6" s="12"/>
       <c r="E6" s="8"/>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
     </row>
     <row r="7" spans="1:10">
       <c r="A7" s="3" t="s">
@@ -1922,11 +1903,9 @@
       <c r="C7" s="7"/>
       <c r="D7" s="12"/>
       <c r="E7" s="8"/>
-      <c r="F7" s="25" t="s">
+      <c r="F7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="25"/>
-      <c r="H7" s="26"/>
     </row>
     <row r="8" spans="1:10">
       <c r="A8" s="3" t="s">
@@ -1934,61 +1913,51 @@
       </c>
       <c r="B8" s="6"/>
       <c r="C8" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="24"/>
+        <v>64</v>
+      </c>
+      <c r="D8" s="22"/>
       <c r="E8" s="11"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="26"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="95" t="s">
+      <c r="A9" s="87" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="96"/>
+      <c r="B9" s="88"/>
       <c r="C9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="24"/>
+      <c r="D9" s="22"/>
       <c r="E9" s="11"/>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="25"/>
-      <c r="H9" s="26"/>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="95" t="s">
+      <c r="A10" s="87" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="96"/>
-      <c r="C10" s="65" t="s">
+      <c r="B10" s="88"/>
+      <c r="C10" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="24"/>
+      <c r="D10" s="22"/>
       <c r="E10" s="11"/>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="25"/>
-      <c r="H10" s="26"/>
     </row>
     <row r="11" spans="1:10" ht="45" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B11" s="6"/>
-      <c r="C11" s="97" t="s">
+      <c r="C11" s="89" t="s">
         <v>60</v>
       </c>
-      <c r="D11" s="98"/>
-      <c r="E11" s="99"/>
-      <c r="F11" s="55"/>
-      <c r="G11" s="55"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
+      <c r="D11" s="90"/>
+      <c r="E11" s="91"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
     </row>
     <row r="12" spans="1:10">
       <c r="A12" s="3" t="s">
@@ -2000,18 +1969,13 @@
       </c>
       <c r="D12" s="12"/>
       <c r="E12" s="8"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-    </row>
-    <row r="13" spans="1:10" s="23" customFormat="1">
-      <c r="A13" s="52" t="s">
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="B13" s="53"/>
-      <c r="C13" s="54" t="s">
+      <c r="B13" s="13"/>
+      <c r="C13" s="45" t="s">
         <v>59</v>
       </c>
       <c r="D13" t="s">
@@ -2019,43 +1983,43 @@
       </c>
       <c r="E13"/>
       <c r="F13"/>
-      <c r="G13" s="56"/>
+      <c r="G13"/>
       <c r="H13"/>
     </row>
-    <row r="14" spans="1:10" s="23" customFormat="1">
-      <c r="A14" s="52" t="s">
+    <row r="14" spans="1:10">
+      <c r="A14" s="44" t="s">
         <v>44</v>
       </c>
-      <c r="B14" s="53"/>
-      <c r="C14" s="54"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="45"/>
       <c r="D14" t="s">
         <v>47</v>
       </c>
       <c r="E14"/>
       <c r="F14"/>
-      <c r="G14" s="56"/>
+      <c r="G14"/>
       <c r="H14"/>
     </row>
-    <row r="15" spans="1:10" s="23" customFormat="1">
-      <c r="A15" s="52" t="s">
+    <row r="15" spans="1:10">
+      <c r="A15" s="44" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="53"/>
-      <c r="C15" s="54" t="s">
+      <c r="B15" s="13"/>
+      <c r="C15" s="45" t="s">
         <v>15</v>
       </c>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
-      <c r="G15" s="56"/>
+      <c r="G15"/>
       <c r="H15"/>
     </row>
-    <row r="16" spans="1:10" s="23" customFormat="1">
-      <c r="A16" s="100" t="s">
+    <row r="16" spans="1:10">
+      <c r="A16" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="B16" s="101"/>
-      <c r="C16" s="54" t="s">
+      <c r="B16" s="93"/>
+      <c r="C16" s="45" t="s">
         <v>15</v>
       </c>
       <c r="D16" t="s">
@@ -2063,516 +2027,487 @@
       </c>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" s="56"/>
+      <c r="G16"/>
       <c r="H16"/>
     </row>
-    <row r="17" spans="1:12" s="28" customFormat="1">
-      <c r="A17" s="25"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="25"/>
-      <c r="D17" s="25"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-    </row>
-    <row r="18" spans="1:12" s="23" customFormat="1">
-      <c r="A18" s="21" t="s">
+    <row r="17" spans="1:12">
+      <c r="B17"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="22"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="22"/>
-      <c r="E18" s="22"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="80"/>
-    </row>
-    <row r="19" spans="1:12" s="23" customFormat="1">
-      <c r="A19" s="81" t="s">
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="70"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="70"/>
-      <c r="C19" s="82"/>
-      <c r="D19" s="82"/>
-      <c r="E19" s="82"/>
-      <c r="F19" s="82"/>
-      <c r="G19" s="83"/>
-      <c r="H19" s="84"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="84"/>
-      <c r="L19" s="84"/>
-    </row>
-    <row r="20" spans="1:12" s="23" customFormat="1">
-      <c r="A20" s="85" t="s">
+      <c r="B19" s="60"/>
+      <c r="C19" s="72"/>
+      <c r="D19" s="72"/>
+      <c r="E19" s="72"/>
+      <c r="F19" s="72"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
+      <c r="L19" s="47"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B20" s="86"/>
-      <c r="C20" s="87"/>
-      <c r="D20" s="88"/>
-      <c r="E20" s="88"/>
-      <c r="F20" s="88"/>
-      <c r="G20" s="89"/>
-    </row>
-    <row r="21" spans="1:12" s="23" customFormat="1">
-      <c r="A21" s="85" t="s">
+      <c r="B20" s="6"/>
+      <c r="C20" s="10"/>
+      <c r="D20" s="22"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="74"/>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B21" s="86"/>
-      <c r="C21" s="90"/>
-      <c r="D21" s="91"/>
-      <c r="E21" s="91"/>
-      <c r="F21" s="91"/>
-      <c r="G21" s="92"/>
-    </row>
-    <row r="22" spans="1:12" s="23" customFormat="1">
+      <c r="B21" s="6"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="75"/>
+    </row>
+    <row r="22" spans="1:12">
       <c r="B22"/>
     </row>
     <row r="23" spans="1:12">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="B23" s="22"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="22"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="35" t="s">
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="52"/>
+      <c r="F23" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G23" s="35"/>
-      <c r="H23" s="35"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="34"/>
-      <c r="K23" s="34"/>
-      <c r="L23" s="34"/>
     </row>
     <row r="24" spans="1:12">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="33" t="s">
+      <c r="B24" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="57"/>
-      <c r="G24" s="57"/>
-      <c r="H24" s="57"/>
-      <c r="I24" s="35"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="26"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="53"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="42">
+      <c r="A25" s="34">
         <v>1</v>
       </c>
-      <c r="B25" s="37" t="s">
+      <c r="B25" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C25" s="29"/>
-      <c r="D25" s="29"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
-      <c r="L25" s="26"/>
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="E25" s="24"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
     </row>
     <row r="26" spans="1:12">
-      <c r="A26" s="42">
+      <c r="A26" s="34">
         <f>A25+1</f>
         <v>2</v>
       </c>
-      <c r="B26" s="37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C26" s="31"/>
-      <c r="D26" s="31"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
-      <c r="L26" s="26"/>
+      <c r="B26" s="29" t="s">
+        <v>63</v>
+      </c>
+      <c r="C26" s="25"/>
+      <c r="D26" s="25"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="48"/>
+      <c r="G26" s="48"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
     </row>
     <row r="27" spans="1:12">
-      <c r="A27" s="42">
-        <f t="shared" ref="A27:A28" si="0">A26+1</f>
+      <c r="A27" s="34">
+        <f t="shared" ref="A27:A29" si="0">A26+1</f>
         <v>3</v>
       </c>
-      <c r="B27" s="37" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" s="31"/>
-      <c r="D27" s="31"/>
-      <c r="E27" s="32"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="27"/>
-      <c r="J27" s="27"/>
-      <c r="K27" s="27"/>
-      <c r="L27" s="26"/>
+      <c r="B27" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="25"/>
+      <c r="D27" s="25"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="48"/>
+      <c r="G27" s="48"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
     </row>
     <row r="28" spans="1:12">
-      <c r="A28" s="42">
+      <c r="A28" s="34">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B28" s="37" t="s">
+      <c r="B28" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C28" s="31"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="32"/>
-      <c r="F28" s="58"/>
-      <c r="G28" s="58"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="27"/>
-      <c r="J28" s="27"/>
-      <c r="K28" s="27"/>
-      <c r="L28" s="26"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="48"/>
+      <c r="G28" s="48"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
     </row>
     <row r="29" spans="1:12">
-      <c r="A29" s="43"/>
-      <c r="B29" s="39"/>
-      <c r="C29" s="40"/>
-      <c r="D29" s="40"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="58"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="27"/>
-      <c r="J29" s="27"/>
-      <c r="K29" s="27"/>
-      <c r="L29" s="26"/>
+      <c r="A29" s="34">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="C29" s="25"/>
+      <c r="D29" s="25"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="48"/>
+      <c r="G29" s="48"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
     </row>
     <row r="30" spans="1:12">
-      <c r="A30" s="64"/>
-      <c r="B30" s="57"/>
-      <c r="C30" s="58"/>
-      <c r="D30" s="58"/>
-      <c r="E30" s="58"/>
-      <c r="F30" s="58"/>
-      <c r="G30" s="58"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="27"/>
-      <c r="J30" s="27"/>
-      <c r="K30" s="27"/>
-      <c r="L30" s="26"/>
+      <c r="A30" s="35"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="32"/>
+      <c r="D30" s="32"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="48"/>
+      <c r="G30" s="48"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
     </row>
     <row r="31" spans="1:12">
-      <c r="A31" s="64"/>
-      <c r="B31" s="57"/>
-      <c r="C31" s="58"/>
-      <c r="D31" s="58"/>
-      <c r="E31" s="58"/>
-      <c r="F31" s="58"/>
-      <c r="G31" s="58"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="27"/>
-      <c r="J31" s="27"/>
-      <c r="K31" s="27"/>
-      <c r="L31" s="26"/>
+      <c r="A31" s="54"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="48"/>
+      <c r="D31" s="48"/>
+      <c r="E31" s="48"/>
+      <c r="F31" s="48"/>
+      <c r="G31" s="48"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
     </row>
     <row r="32" spans="1:12">
-      <c r="A32" s="21" t="s">
+      <c r="A32" s="54"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="48"/>
+      <c r="E32" s="48"/>
+      <c r="F32" s="48"/>
+      <c r="G32" s="48"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="B32" s="22"/>
-      <c r="C32" s="22"/>
-      <c r="D32" s="22"/>
-      <c r="E32" s="22"/>
-      <c r="F32" s="62"/>
-      <c r="G32" s="35" t="s">
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="52"/>
+      <c r="G33" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H32" s="35"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="34"/>
-    </row>
-    <row r="33" spans="1:12">
-      <c r="A33" s="38" t="s">
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B33" s="33" t="s">
+      <c r="B34" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="70"/>
-      <c r="F33" s="66" t="s">
+      <c r="C34" s="27"/>
+      <c r="D34" s="27"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="56" t="s">
         <v>43</v>
       </c>
-      <c r="G33" s="57"/>
-      <c r="H33" s="57"/>
-      <c r="I33" s="35"/>
-      <c r="J33" s="36"/>
-      <c r="K33" s="36"/>
-      <c r="L33" s="26"/>
-    </row>
-    <row r="34" spans="1:12">
-      <c r="A34" s="42"/>
-      <c r="B34" s="37"/>
-      <c r="C34" s="29"/>
-      <c r="D34" s="29"/>
-      <c r="E34" s="71"/>
-      <c r="F34" s="68"/>
-      <c r="G34" s="58"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="27"/>
-      <c r="J34" s="27"/>
-      <c r="K34" s="27"/>
-      <c r="L34" s="26"/>
+      <c r="G34" s="47"/>
+      <c r="H34" s="47"/>
+      <c r="J34" s="28"/>
+      <c r="K34" s="28"/>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="42"/>
-      <c r="B35" s="37"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="72"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="58"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="27"/>
-      <c r="J35" s="27"/>
-      <c r="K35" s="27"/>
-      <c r="L35" s="26"/>
+      <c r="A35" s="34"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
+      <c r="E35" s="61"/>
+      <c r="F35" s="58"/>
+      <c r="G35" s="48"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="43"/>
-      <c r="B36" s="39"/>
-      <c r="C36" s="40"/>
-      <c r="D36" s="40"/>
-      <c r="E36" s="73"/>
-      <c r="F36" s="67"/>
-      <c r="G36" s="58"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="27"/>
-      <c r="J36" s="27"/>
-      <c r="K36" s="27"/>
-      <c r="L36" s="26"/>
+      <c r="A36" s="34"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="25"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="62"/>
+      <c r="F36" s="59"/>
+      <c r="G36" s="48"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
     </row>
     <row r="37" spans="1:12">
-      <c r="A37" s="64"/>
-      <c r="B37" s="57"/>
-      <c r="C37" s="58"/>
-      <c r="D37" s="58"/>
-      <c r="E37" s="58"/>
-      <c r="F37" s="58"/>
-      <c r="G37" s="58"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="27"/>
-      <c r="J37" s="27"/>
-      <c r="K37" s="27"/>
-      <c r="L37" s="26"/>
+      <c r="A37" s="35"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="63"/>
+      <c r="F37" s="57"/>
+      <c r="G37" s="48"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13" t="s">
+      <c r="A38" s="54"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="48"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="48"/>
+      <c r="F38" s="48"/>
+      <c r="G38" s="48"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39"/>
+      <c r="B39" t="s">
         <v>46</v>
       </c>
-      <c r="C38" s="13"/>
-      <c r="D38" s="13"/>
-      <c r="E38" s="13"/>
-      <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
-      <c r="I38" s="13"/>
-    </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="3" t="s">
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B39" s="14"/>
-      <c r="C39" s="14"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="14"/>
-      <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="14"/>
-      <c r="I39" s="14"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="15"/>
-    </row>
-    <row r="40" spans="1:12" ht="13.5" customHeight="1">
-      <c r="A40" s="103" t="s">
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
+      <c r="D40" s="13"/>
+      <c r="E40" s="13"/>
+      <c r="F40" s="13"/>
+      <c r="G40" s="13"/>
+      <c r="H40" s="13"/>
+      <c r="I40" s="13"/>
+      <c r="J40" s="13"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="14"/>
+    </row>
+    <row r="41" spans="1:12" ht="13.5" customHeight="1">
+      <c r="A41" s="95" t="s">
         <v>8</v>
       </c>
-      <c r="B40" s="103" t="s">
+      <c r="B41" s="95" t="s">
         <v>3</v>
       </c>
-      <c r="C40" s="102" t="s">
+      <c r="C41" s="94" t="s">
         <v>4</v>
       </c>
-      <c r="D40" s="102" t="s">
+      <c r="D41" s="94" t="s">
         <v>6</v>
       </c>
-      <c r="E40" s="102" t="s">
+      <c r="E41" s="94" t="s">
         <v>5</v>
       </c>
-      <c r="F40" s="104" t="s">
+      <c r="F41" s="96" t="s">
         <v>26</v>
       </c>
-      <c r="G40" s="104" t="s">
+      <c r="G41" s="96" t="s">
         <v>17</v>
       </c>
-      <c r="H40" s="102" t="s">
+      <c r="H41" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="I40" s="102"/>
-      <c r="J40" s="16"/>
-      <c r="K40" s="17"/>
-      <c r="L40" s="9"/>
-    </row>
-    <row r="41" spans="1:12">
-      <c r="A41" s="103"/>
-      <c r="B41" s="103"/>
-      <c r="C41" s="102"/>
-      <c r="D41" s="102"/>
-      <c r="E41" s="102"/>
-      <c r="F41" s="105"/>
-      <c r="G41" s="105"/>
-      <c r="H41" s="102"/>
-      <c r="I41" s="102"/>
-      <c r="J41" s="18"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="15"/>
-    </row>
-    <row r="42" spans="1:12" ht="32" customHeight="1">
-      <c r="A42" s="19"/>
-      <c r="B42" s="59"/>
-      <c r="C42" s="59"/>
-      <c r="D42" s="74"/>
-      <c r="E42" s="74"/>
-      <c r="F42" s="74"/>
-      <c r="G42" s="75"/>
-      <c r="H42" s="112"/>
-      <c r="I42" s="113"/>
-      <c r="J42" s="113"/>
-      <c r="K42" s="114"/>
-      <c r="L42" s="15"/>
-    </row>
-    <row r="43" spans="1:12">
-      <c r="A43" s="19"/>
-      <c r="B43" s="59"/>
-      <c r="C43" s="59"/>
-      <c r="D43" s="74"/>
-      <c r="E43" s="74"/>
-      <c r="F43" s="74"/>
-      <c r="G43" s="75"/>
-      <c r="H43" s="106"/>
-      <c r="I43" s="107"/>
-      <c r="J43" s="107"/>
-      <c r="K43" s="108"/>
-      <c r="L43" s="15"/>
+      <c r="I41" s="94"/>
+      <c r="J41" s="15"/>
+      <c r="K41" s="16"/>
+      <c r="L41" s="9"/>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="95"/>
+      <c r="B42" s="95"/>
+      <c r="C42" s="94"/>
+      <c r="D42" s="94"/>
+      <c r="E42" s="94"/>
+      <c r="F42" s="97"/>
+      <c r="G42" s="97"/>
+      <c r="H42" s="94"/>
+      <c r="I42" s="94"/>
+      <c r="J42" s="17"/>
+      <c r="K42" s="19"/>
+      <c r="L42" s="14"/>
+    </row>
+    <row r="43" spans="1:12" ht="32" customHeight="1">
+      <c r="A43" s="18"/>
+      <c r="B43" s="49"/>
+      <c r="C43" s="49"/>
+      <c r="D43" s="64"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="64"/>
+      <c r="G43" s="65"/>
+      <c r="H43" s="84"/>
+      <c r="I43" s="85"/>
+      <c r="J43" s="85"/>
+      <c r="K43" s="86"/>
+      <c r="L43" s="14"/>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="19"/>
-      <c r="B44" s="60"/>
-      <c r="C44" s="60"/>
-      <c r="D44" s="74"/>
-      <c r="E44" s="74"/>
-      <c r="F44" s="74"/>
-      <c r="G44" s="75"/>
-      <c r="H44" s="106"/>
-      <c r="I44" s="107"/>
-      <c r="J44" s="107"/>
-      <c r="K44" s="108"/>
-      <c r="L44" s="15"/>
+      <c r="A44" s="18"/>
+      <c r="B44" s="49"/>
+      <c r="C44" s="49"/>
+      <c r="D44" s="64"/>
+      <c r="E44" s="64"/>
+      <c r="F44" s="64"/>
+      <c r="G44" s="65"/>
+      <c r="H44" s="78"/>
+      <c r="I44" s="79"/>
+      <c r="J44" s="79"/>
+      <c r="K44" s="80"/>
+      <c r="L44" s="14"/>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="19"/>
-      <c r="B45" s="61"/>
-      <c r="C45" s="61"/>
-      <c r="D45" s="74"/>
-      <c r="E45" s="74"/>
-      <c r="F45" s="74"/>
-      <c r="G45" s="75"/>
-      <c r="H45" s="106"/>
-      <c r="I45" s="107"/>
-      <c r="J45" s="107"/>
-      <c r="K45" s="108"/>
-      <c r="L45" s="15"/>
+      <c r="A45" s="18"/>
+      <c r="B45" s="50"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="64"/>
+      <c r="F45" s="64"/>
+      <c r="G45" s="65"/>
+      <c r="H45" s="78"/>
+      <c r="I45" s="79"/>
+      <c r="J45" s="79"/>
+      <c r="K45" s="80"/>
+      <c r="L45" s="14"/>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="19"/>
-      <c r="B46" s="61"/>
-      <c r="C46" s="61"/>
-      <c r="D46" s="74"/>
-      <c r="E46" s="74"/>
-      <c r="F46" s="74"/>
-      <c r="G46" s="75"/>
-      <c r="H46" s="106"/>
-      <c r="I46" s="107"/>
-      <c r="J46" s="107"/>
-      <c r="K46" s="108"/>
-      <c r="L46" s="15"/>
+      <c r="A46" s="18"/>
+      <c r="B46" s="51"/>
+      <c r="C46" s="51"/>
+      <c r="D46" s="64"/>
+      <c r="E46" s="64"/>
+      <c r="F46" s="64"/>
+      <c r="G46" s="65"/>
+      <c r="H46" s="78"/>
+      <c r="I46" s="79"/>
+      <c r="J46" s="79"/>
+      <c r="K46" s="80"/>
+      <c r="L46" s="14"/>
     </row>
     <row r="47" spans="1:12">
-      <c r="A47" s="19"/>
-      <c r="B47" s="61"/>
-      <c r="C47" s="61"/>
-      <c r="D47" s="37"/>
-      <c r="E47" s="37"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="76"/>
-      <c r="H47" s="106"/>
-      <c r="I47" s="107"/>
-      <c r="J47" s="107"/>
-      <c r="K47" s="108"/>
-      <c r="L47" s="15"/>
+      <c r="A47" s="18"/>
+      <c r="B47" s="51"/>
+      <c r="C47" s="51"/>
+      <c r="D47" s="64"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="64"/>
+      <c r="G47" s="65"/>
+      <c r="H47" s="78"/>
+      <c r="I47" s="79"/>
+      <c r="J47" s="79"/>
+      <c r="K47" s="80"/>
+      <c r="L47" s="14"/>
     </row>
     <row r="48" spans="1:12">
-      <c r="A48" s="77"/>
-      <c r="B48" s="78"/>
-      <c r="C48" s="39"/>
-      <c r="D48" s="39"/>
-      <c r="E48" s="39"/>
-      <c r="F48" s="39"/>
-      <c r="G48" s="79"/>
-      <c r="H48" s="109"/>
-      <c r="I48" s="110"/>
-      <c r="J48" s="110"/>
-      <c r="K48" s="111"/>
-      <c r="L48" s="15"/>
+      <c r="A48" s="18"/>
+      <c r="B48" s="51"/>
+      <c r="C48" s="51"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="29"/>
+      <c r="G48" s="66"/>
+      <c r="H48" s="78"/>
+      <c r="I48" s="79"/>
+      <c r="J48" s="79"/>
+      <c r="K48" s="80"/>
+      <c r="L48" s="14"/>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="67"/>
+      <c r="B49" s="68"/>
+      <c r="C49" s="31"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="31"/>
+      <c r="G49" s="69"/>
+      <c r="H49" s="81"/>
+      <c r="I49" s="82"/>
+      <c r="J49" s="82"/>
+      <c r="K49" s="83"/>
+      <c r="L49" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="H47:K47"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H41:I42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="E41:E42"/>
+    <mergeCell ref="D41:D42"/>
+    <mergeCell ref="G41:G42"/>
+    <mergeCell ref="F41:F42"/>
     <mergeCell ref="H48:K48"/>
-    <mergeCell ref="H42:K42"/>
+    <mergeCell ref="H49:K49"/>
     <mergeCell ref="H43:K43"/>
     <mergeCell ref="H44:K44"/>
     <mergeCell ref="H45:K45"/>
     <mergeCell ref="H46:K46"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H40:I41"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="E40:E41"/>
-    <mergeCell ref="D40:D41"/>
-    <mergeCell ref="G40:G41"/>
-    <mergeCell ref="F40:F41"/>
+    <mergeCell ref="H47:K47"/>
   </mergeCells>
   <phoneticPr fontId="3"/>
   <dataValidations count="5">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E64:G64" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E65:G65" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>型</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2585,7 +2520,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C14:C15" xr:uid="{CCFC1331-CEEF-574E-9BCC-37D38F486896}">
       <formula1>adjustFieldName</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F42:G48" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F43:G49" xr:uid="{18C70D90-9F1A-D84D-9F1C-490DE84E2C64}">
       <formula1>yesNo</formula1>
     </dataValidation>
   </dataValidations>
@@ -2610,84 +2545,84 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="3" width="8.83203125" style="46" customWidth="1"/>
-    <col min="4" max="4" width="9.83203125" style="46" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="46" customWidth="1"/>
-    <col min="6" max="6" width="18.5" style="46" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.83203125" style="46" customWidth="1"/>
-    <col min="8" max="8" width="18.6640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="46" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" style="46" bestFit="1" customWidth="1"/>
-    <col min="11" max="251" width="8.83203125" style="46" customWidth="1"/>
-    <col min="252" max="16384" width="10.83203125" style="46"/>
+    <col min="1" max="3" width="8.83203125" style="38" customWidth="1"/>
+    <col min="4" max="4" width="9.83203125" style="38" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" style="38" customWidth="1"/>
+    <col min="6" max="6" width="18.5" style="38" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="38" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="38" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" style="38" bestFit="1" customWidth="1"/>
+    <col min="11" max="251" width="8.83203125" style="38" customWidth="1"/>
+    <col min="252" max="16384" width="10.83203125" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="19">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="45" t="s">
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="37" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="39" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="47" t="s">
+      <c r="D3" s="39" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="47" t="s">
+      <c r="H3" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="47" t="s">
+      <c r="J3" s="39" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="J4" s="49"/>
+      <c r="F4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="J4" s="41"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="B5" s="93" t="s">
+      <c r="B5" s="76" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="51"/>
-      <c r="F5" s="51" t="s">
+      <c r="D5" s="43"/>
+      <c r="F5" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="H5" s="51" t="s">
+      <c r="H5" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="J5" s="51" t="s">
+      <c r="J5" s="43" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="B6" s="94" t="s">
+      <c r="B6" s="77" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="B7" s="50" t="s">
+      <c r="B7" s="42" t="s">
         <v>57</v>
       </c>
     </row>

</xml_diff>